<commit_message>
update export excel format
</commit_message>
<xml_diff>
--- a/front/src/assets/template0.xlsx
+++ b/front/src/assets/template0.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26666102-8C26-1F49-BC60-8F6195E9D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D65EAC-4086-9B41-B65A-06B914EBFF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="40" windowWidth="25440" windowHeight="14580" xr2:uid="{76C8A18E-85FC-7F4F-A75C-062BA0A56423}"/>
   </bookViews>
   <sheets>
-    <sheet name="MAGISTRATS" sheetId="2" r:id="rId1"/>
-    <sheet name="FONCTIONNAIRES" sheetId="3" r:id="rId2"/>
+    <sheet name="NOTICE et COMMENTAIRES" sheetId="4" r:id="rId1"/>
+    <sheet name="MAGISTRATS" sheetId="2" r:id="rId2"/>
+    <sheet name="FONCTIONNAIRES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>Template d'import pour référentiel de temps moyen A-JUST</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Identifiant</t>
   </si>
@@ -91,6 +89,14 @@
   </si>
   <si>
     <t>## y.averageProcessingTimeFonc</t>
+  </si>
+  <si>
+    <t>#` Export d'un référentiel de temps moyens A-JUST : ${name} 
+(ce fichier peut être importé directement dans A-JUST)</t>
+  </si>
+  <si>
+    <t>#` Export d'un référentiel de temps moyens A-JUST : ${nameFonc} 
+(ce fichier peut être importé directement dans A-JUST)</t>
   </si>
 </sst>
 </file>
@@ -177,13 +183,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,74 +503,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636CCCC4-63F1-4D4E-85CC-3ED9A3EFA513}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB31E4F-D62C-BB4D-B976-6FFEE4FE1739}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
+    <row r="1" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7"/>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -575,75 +599,75 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E006FAA4-051D-854A-B9F2-9E0E6ABF8555}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
+    <row r="1" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7"/>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add notice et commentaire
</commit_message>
<xml_diff>
--- a/front/src/assets/template0.xlsx
+++ b/front/src/assets/template0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D65EAC-4086-9B41-B65A-06B914EBFF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FE6195-F750-2649-9C4E-E34FA047D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="40" windowWidth="25440" windowHeight="14580" xr2:uid="{76C8A18E-85FC-7F4F-A75C-062BA0A56423}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Identifiant</t>
   </si>
@@ -97,6 +97,201 @@
   <si>
     <t>#` Export d'un référentiel de temps moyens A-JUST : ${nameFonc} 
 (ce fichier peut être importé directement dans A-JUST)</t>
+  </si>
+  <si>
+    <t>Ce fichier résulte de l'export d'un référentiel de temps moyens depuis l'onglet "Temps moyens" d'A-JUST</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dans l'onglet "MAGISTRATS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, vous trouverez les temps moyens par dossier enregistrés dans ce référentiel pour les magistrats, pour chacun des contentieux et sous-contentieux.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A l'identique, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dans l'onglet "FONCTIONNAIRES"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, vous trouverez les temps moyens enregistrés pour les agents du greffe.</t>
+    </r>
+  </si>
+  <si>
+    <t>Les temps sont indiqués en heures et minutes, selon le format "h:mm", c’est-à-dire 3:26 pour 3 heures et 26 minutes ou 2:01 pour 2 heures et 1 minute.</t>
+  </si>
+  <si>
+    <t>Vous pouvez créer un nouveau référentiel A-JUST directement dans l'outil, en partant d'une base vierge ou en dupliquant un référentiel existant (fonctionnalités disponibles dans le menu "Options").</t>
+  </si>
+  <si>
+    <t>Vous pouvez également faire évoluer à tout moment un référentiel existant en modifiant les données présentes à l'écran puis en cliquant sur "enregistrer" (ou "enregistrer sous" pour l'enregistrer sous un nouveau nom).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toutefois, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>si vous souhaitez utiliser ce fichier pour créer un nouveau référentiel dans A-JUST, notamment s'il vous a été transmis, vous pouvez l'importer tel quel ou le modifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L'import s'effectue dans A-JUST en utilisant la fonction</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Importer"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dans le menu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Options"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> puis en sélectionnant le fichier sur le disque dur de votre ordinateur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Au moment de l'import, A-JUST vous demandera le nom que vous souhaitez donner à ce nouveau référentiel de temps moyens et vous le retrouverez dans le menu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Mes temps moyens de comparaison"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> situé en haut de l'écran.</t>
+    </r>
+  </si>
+  <si>
+    <t>Précautions d'usage :</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si vous modifiez ce référentiel de temps moyens dans excel, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>il est essentiel de ne modifier ni la structure du fichier, ni le format des données</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : veillez à ne pas supprimer d'onglet ni de ligne et à respecter le format "h:mm"</t>
+    </r>
+  </si>
+  <si>
+    <t>Si vous souhaitez ne pas importer de temps moyens par dossier pour les fonctionnaires (ou pour les magistrats), ne supprimez pas l'onglet correspondant mais effacez le contenu de toutes les cellules.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI vous souhaitez saisir un temps de 3 heures et 4 minutes, il vous faut noter "3:04" et pas "3:4" ni "03:04". </t>
   </si>
 </sst>
 </file>
@@ -106,7 +301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.###;0.###;\-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,6 +320,38 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,6 +416,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,14 +758,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636CCCC4-63F1-4D4E-85CC-3ED9A3EFA513}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="161.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:2" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -525,7 +939,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished onglet temps moyen
</commit_message>
<xml_diff>
--- a/front/src/assets/template0.xlsx
+++ b/front/src/assets/template0.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FE6195-F750-2649-9C4E-E34FA047D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F1ED6C-CF05-DA48-96F8-219ABCBAE8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="40" windowWidth="25440" windowHeight="14580" xr2:uid="{76C8A18E-85FC-7F4F-A75C-062BA0A56423}"/>
+    <workbookView xWindow="80" yWindow="760" windowWidth="25440" windowHeight="14580" xr2:uid="{76C8A18E-85FC-7F4F-A75C-062BA0A56423}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTICE et COMMENTAIRES" sheetId="4" r:id="rId1"/>
-    <sheet name="MAGISTRATS" sheetId="2" r:id="rId2"/>
-    <sheet name="FONCTIONNAIRES" sheetId="3" r:id="rId3"/>
+    <sheet name="TEMPS-MOYENS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Identifiant</t>
   </si>
@@ -70,85 +69,10 @@
     <t>#! FOR_EACH x referentiels</t>
   </si>
   <si>
-    <t>#! FOR_EACH y referentielsFonc</t>
-  </si>
-  <si>
-    <t>#! CONTINUE y</t>
-  </si>
-  <si>
-    <t>#! END_LOOP y</t>
-  </si>
-  <si>
-    <t>## y.label</t>
-  </si>
-  <si>
-    <t>## y.id</t>
-  </si>
-  <si>
     <t>## x.averageProcessingTime</t>
   </si>
   <si>
-    <t>## y.averageProcessingTimeFonc</t>
-  </si>
-  <si>
-    <t>#` Export d'un référentiel de temps moyens A-JUST : ${name} 
-(ce fichier peut être importé directement dans A-JUST)</t>
-  </si>
-  <si>
-    <t>#` Export d'un référentiel de temps moyens A-JUST : ${nameFonc} 
-(ce fichier peut être importé directement dans A-JUST)</t>
-  </si>
-  <si>
     <t>Ce fichier résulte de l'export d'un référentiel de temps moyens depuis l'onglet "Temps moyens" d'A-JUST</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dans l'onglet "MAGISTRATS"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, vous trouverez les temps moyens par dossier enregistrés dans ce référentiel pour les magistrats, pour chacun des contentieux et sous-contentieux.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A l'identique, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dans l'onglet "FONCTIONNAIRES"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, vous trouverez les temps moyens enregistrés pour les agents du greffe.</t>
-    </r>
   </si>
   <si>
     <t>Les temps sont indiqués en heures et minutes, selon le format "h:mm", c’est-à-dire 3:26 pour 3 heures et 26 minutes ou 2:01 pour 2 heures et 1 minute.</t>
@@ -233,32 +157,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Au moment de l'import, A-JUST vous demandera le nom que vous souhaitez donner à ce nouveau référentiel de temps moyens et vous le retrouverez dans le menu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Mes temps moyens de comparaison"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> situé en haut de l'écran.</t>
-    </r>
-  </si>
-  <si>
     <t>Précautions d'usage :</t>
   </si>
   <si>
@@ -292,6 +190,36 @@
   </si>
   <si>
     <t xml:space="preserve">SI vous souhaitez saisir un temps de 3 heures et 4 minutes, il vous faut noter "3:04" et pas "3:4" ni "03:04". </t>
+  </si>
+  <si>
+    <t>#` Export d'un référentiel de temps moyens A-JUST 
+(ce fichier peut être importé directement dans A-JUST)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dans l'onglet "TEMPS-MOYENS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, vous trouverez les temps moyens par dossier enregistrés dans ce référentiel, pour chacun des contentieux et sous-contentieux.</t>
+    </r>
+  </si>
+  <si>
+    <t>Au moment de l'import, A-JUST vous demandera le nom que vous souhaitez donner à ce nouveau référentiel de temps moyens et vous le retrouverez dans la liste de vos référentiels de temps-moyen.</t>
   </si>
 </sst>
 </file>
@@ -414,35 +342,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,9 +390,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +430,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -608,7 +536,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,7 +678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -758,174 +686,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636CCCC4-63F1-4D4E-85CC-3ED9A3EFA513}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="161.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="11"/>
+    <col min="1" max="1" width="161.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>19</v>
+      <c r="A1" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:15" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:15" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="13" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="13" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="13" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="13" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:2" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -936,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB31E4F-D62C-BB4D-B976-6FFEE4FE1739}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,10 +868,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16"/>
       <c r="D1" t="s">
         <v>3</v>
       </c>
@@ -980,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -994,94 +912,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E006FAA4-051D-854A-B9F2-9E0E6ABF8555}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>